<commit_message>
Started to crawl the tldr-corpus.
</commit_message>
<xml_diff>
--- a/Database/documentation.xlsx
+++ b/Database/documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3826F1AC-3EFB-4F09-9CD0-176E063003B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCC3DD4-72F4-485E-B23B-CE91BF702E76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="165" windowWidth="21405" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="165" windowWidth="21405" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -61,6 +61,24 @@
   </si>
   <si>
     <t>EN</t>
+  </si>
+  <si>
+    <t>TLDR</t>
+  </si>
+  <si>
+    <t>Branche</t>
+  </si>
+  <si>
+    <t>Wiki</t>
+  </si>
+  <si>
+    <t>Recht</t>
+  </si>
+  <si>
+    <t>News</t>
+  </si>
+  <si>
+    <t>Social</t>
   </si>
 </sst>
 </file>
@@ -390,17 +408,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="2" max="6" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,98 +426,136 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E2" s="2">
         <v>2.17</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>263000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="2">
         <v>0.53</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>157252</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="2">
         <v>1.27</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>287113</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
         <v>1</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="2">
         <v>1.07</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3803113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>11.8</v>
+      </c>
+      <c r="F7">
+        <v>4000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>